<commit_message>
Claudia Kommentare - bis inkl. 31
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -8,15 +8,16 @@
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
-    <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
+    <sheet name="14bis18" sheetId="2" r:id="rId2"/>
+    <sheet name="19bis20" sheetId="3" r:id="rId3"/>
+    <sheet name="21bis26" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="63">
   <si>
     <t>Nr.</t>
   </si>
@@ -138,19 +139,73 @@
     <t>Font Menü: Source Sans Pro REGULAR / Farbe schwarz</t>
   </si>
   <si>
-    <t>Farbe angepasst - Font war korrekt</t>
-  </si>
-  <si>
     <t>Font Menü: Source Sans Pro REGULAR / Farbe 30/50/104</t>
   </si>
   <si>
-    <t xml:space="preserve"> Farbe 135/142/171</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Farbe angepasst </t>
-  </si>
-  <si>
     <t>Menü linksbündig</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Farbe 135/142/171 / Groß-Kleinschreibung</t>
+  </si>
+  <si>
+    <t>Farbe angepasst / Großschreibung angepasst</t>
+  </si>
+  <si>
+    <t>Mouseover blau</t>
+  </si>
+  <si>
+    <t>Nach links verschoben</t>
+  </si>
+  <si>
+    <t>Transparente Fläche 70% blau</t>
+  </si>
+  <si>
+    <t>Textfarbe + Mouseover Unterstrich entfernt</t>
+  </si>
+  <si>
+    <t>Farbe blau</t>
+  </si>
+  <si>
+    <t>Lauftext</t>
+  </si>
+  <si>
+    <t>Hintergrundfarbe angepasst</t>
+  </si>
+  <si>
+    <t>Abstand beachten</t>
+  </si>
+  <si>
+    <t>24a</t>
+  </si>
+  <si>
+    <t>HOME / Impressum</t>
+  </si>
+  <si>
+    <t>e-mail Adresse angepasst und vereinheitlicht</t>
+  </si>
+  <si>
+    <t>Herbert</t>
+  </si>
+  <si>
+    <t>in Review</t>
+  </si>
+  <si>
+    <t>Font/Farbe/Mouseover</t>
+  </si>
+  <si>
+    <t>Hintergrundfarbe / Browserfenster</t>
+  </si>
+  <si>
+    <t>Font</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Font/Farbe </t>
+  </si>
+  <si>
+    <t>Hintergrund, Text linksbündig</t>
+  </si>
+  <si>
+    <t>Abstand bei mobiler Ansicht</t>
   </si>
 </sst>
 </file>
@@ -233,6 +288,186 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="11323320" cy="5151120"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>68580</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="11163300" cy="3108960"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>640080</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10942320" cy="6019800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -438,10 +673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -720,86 +955,333 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
+    <row r="15" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
         <v>14</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="B15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="1" t="s">
+      <c r="D15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
-        <v>16</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
-        <v>17</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
-        <v>18</v>
+      <c r="D19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
+        <v>23</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <v>24</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
+        <v>25</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
+        <v>26</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
+        <v>27</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="3">
+        <v>28</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="3">
+        <v>29</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="3">
+        <v>30</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="3">
+        <v>31</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -819,10 +1301,26 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -831,5 +1329,6 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Claudia Kommentare - bis inkl. 38
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -11,13 +11,15 @@
     <sheet name="14bis18" sheetId="2" r:id="rId2"/>
     <sheet name="19bis20" sheetId="3" r:id="rId3"/>
     <sheet name="21bis26" sheetId="4" r:id="rId4"/>
+    <sheet name="27bis31" sheetId="5" r:id="rId5"/>
+    <sheet name="32bis34" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="68">
   <si>
     <t>Nr.</t>
   </si>
@@ -206,6 +208,21 @@
   </si>
   <si>
     <t>Abstand bei mobiler Ansicht</t>
+  </si>
+  <si>
+    <t>Ausrichtung</t>
+  </si>
+  <si>
+    <t>hab versucht es zu optimieren. Es ist mir nicht auf Anhieb gelungen es auf gleicher Größe zu halten, müsste noch um einiges mehr an Zeit investieren. Schaut auch bitte die Lösung an und sagt mir Bescheid.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TÄTIGKEIT </t>
+  </si>
+  <si>
+    <t>Font/Farbe</t>
+  </si>
+  <si>
+    <t>Hintergrundfarbe</t>
   </si>
 </sst>
 </file>
@@ -470,6 +487,126 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="11361420" cy="6294120"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>655320</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10957560" cy="6141720"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="BRZCorporateDesignTheme">
   <a:themeElements>
@@ -673,10 +810,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37:E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1267,7 +1404,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>31</v>
       </c>
@@ -1281,6 +1418,128 @@
         <v>35</v>
       </c>
       <c r="E33" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="3">
+        <v>32</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="3">
+        <v>33</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="3">
+        <v>34</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="3">
+        <v>35</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="3">
+        <v>36</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="3">
+        <v>37</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="3">
+        <v>38</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E40" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1331,4 +1590,32 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Forrest Kommentare bis 41
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="77">
   <si>
     <t>Nr.</t>
   </si>
@@ -223,13 +223,40 @@
   </si>
   <si>
     <t>Hintergrundfarbe</t>
+  </si>
+  <si>
+    <t>Das große Bild (z.B. bei Home) ist gegenüber dem Entwurf von Claudia etwas zusammengestaucht. Kann man das anpassen?</t>
+  </si>
+  <si>
+    <t>in Arbeit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forrest  </t>
+  </si>
+  <si>
+    <t>Das Bild hat ein gewisses Verhältnis Höhe / Breite. Dieses ist vorgegeben. Wenn das Bild weniger verzerrt sein soll, muss entweder die Höhe oder die Breite angepasst werden. Beides hat Impact auf die gesamte Seite. Ersuche um Rückmeldung, wie hoch bzw. wie breit das Pixmap sein soll. Anmerkung: die Devices (Handy, Ipad, ...) haben alle unterschiedliche Verhältnisse - schaut es auf einem "optimal" aus, kann es am anderen nicht gut aussehen. Am PC kann die Fensterbreite des Browsers beliebig eingestellt werden...</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Bei „International“ ist das Logo gegenüber den anderen Seiten größer. Ist mE zu groß, besser wie bei den anderen Seiten.</t>
+  </si>
+  <si>
+    <t>Forrest</t>
+  </si>
+  <si>
+    <t>Kann man auf der Seite „Team“ die Fotos ein bisschen kleiner machen, damit man ein paar mehr Leute sieht?</t>
+  </si>
+  <si>
+    <t>auf 80% gesetzt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,8 +264,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1F497D"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -248,6 +282,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -279,7 +319,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -288,6 +328,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -802,7 +848,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -810,16 +856,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37:E40"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43:XFD43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="56.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="66.109375" style="1" bestFit="1" customWidth="1"/>
@@ -1543,8 +1589,71 @@
         <v>8</v>
       </c>
     </row>
+    <row r="41" spans="1:6" s="4" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A41" s="4">
+        <v>39</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A42" s="3">
+        <v>40</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A43" s="3">
+        <v>41</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F45" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <webPublishItems count="1">
     <webPublishItem id="27866" divId="todo_27866" sourceType="sheet" destinationFile="C:\Entwicklung\projects\gsplegal\gsplegalAngular7\todo.htm"/>
   </webPublishItems>

</xml_diff>

<commit_message>
Forrest Kommentare bis 43
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="79">
   <si>
     <t>Nr.</t>
   </si>
@@ -237,9 +237,6 @@
     <t>Das Bild hat ein gewisses Verhältnis Höhe / Breite. Dieses ist vorgegeben. Wenn das Bild weniger verzerrt sein soll, muss entweder die Höhe oder die Breite angepasst werden. Beides hat Impact auf die gesamte Seite. Ersuche um Rückmeldung, wie hoch bzw. wie breit das Pixmap sein soll. Anmerkung: die Devices (Handy, Ipad, ...) haben alle unterschiedliche Verhältnisse - schaut es auf einem "optimal" aus, kann es am anderen nicht gut aussehen. Am PC kann die Fensterbreite des Browsers beliebig eingestellt werden...</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Bei „International“ ist das Logo gegenüber den anderen Seiten größer. Ist mE zu groß, besser wie bei den anderen Seiten.</t>
   </si>
   <si>
@@ -250,6 +247,15 @@
   </si>
   <si>
     <t>auf 80% gesetzt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Auf der Seite „Home“ ist noch der alte Text (Nischenplayer, etc.). Könntest Du bitte den neuen Text von Claudia’s Konzept nehmen?</t>
+  </si>
+  <si>
+    <t>Deutsch erledigt - Englisch fehlt</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bei „International“ fehlt noch der Text. Den haben wir noch nicht gedraftet. Wie wäre es vorläufig mit:</t>
   </si>
 </sst>
 </file>
@@ -848,7 +854,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -859,7 +865,7 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43:XFD43"/>
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -964,7 +970,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1617,13 +1623,13 @@
         <v>19</v>
       </c>
       <c r="C42" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E42" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="43" spans="1:6" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -1634,21 +1640,56 @@
         <v>9</v>
       </c>
       <c r="C43" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F43" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="F43" s="3" t="s">
+    </row>
+    <row r="44" spans="1:6" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="4">
+        <v>42</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F45" s="1" t="s">
-        <v>72</v>
+      <c r="D44" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="4">
+        <v>43</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Forrest Kommentare per Mail
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -246,9 +246,6 @@
     <t>Kann man auf der Seite „Team“ die Fotos ein bisschen kleiner machen, damit man ein paar mehr Leute sieht?</t>
   </si>
   <si>
-    <t>auf 80% gesetzt</t>
-  </si>
-  <si>
     <t xml:space="preserve">  Auf der Seite „Home“ ist noch der alte Text (Nischenplayer, etc.). Könntest Du bitte den neuen Text von Claudia’s Konzept nehmen?</t>
   </si>
   <si>
@@ -256,6 +253,9 @@
   </si>
   <si>
     <t xml:space="preserve"> Bei „International“ fehlt noch der Text. Den haben wir noch nicht gedraftet. Wie wäre es vorläufig mit:</t>
+  </si>
+  <si>
+    <t>auf 60% gesetzt</t>
   </si>
 </sst>
 </file>
@@ -854,7 +854,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -865,7 +865,7 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1649,7 +1649,7 @@
         <v>73</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="44" spans="1:6" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -1660,7 +1660,7 @@
         <v>4</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>69</v>
@@ -1669,7 +1669,7 @@
         <v>73</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="45" spans="1:6" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -1680,7 +1680,7 @@
         <v>19</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>69</v>
@@ -1689,7 +1689,7 @@
         <v>73</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>